<commit_message>
macrobuilders for linkam and double wheel
camera usb port
move to ws3
more work on linkam interface
</commit_message>
<xml_diff>
--- a/startup/linkam_template.xlsx
+++ b/startup/linkam_template.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BR</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t xml:space="preserve">Linkam</t>
   </si>
@@ -188,9 +188,6 @@
     <t xml:space="preserve">CIF</t>
   </si>
   <si>
-    <t xml:space="preserve">Default</t>
-  </si>
-  <si>
     <t xml:space="preserve">best_sample_ever</t>
   </si>
   <si>
@@ -248,7 +245,7 @@
     <t xml:space="preserve">Cell identifying spreadsheet version number</t>
   </si>
   <si>
-    <t xml:space="preserve">Linkam, double wheel</t>
+    <t xml:space="preserve">Linkam, double wheel, added Ca ans Sc to element column validity</t>
   </si>
 </sst>
 </file>
@@ -896,9 +893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -907,8 +904,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3191040" y="3926160"/>
-          <a:ext cx="6642360" cy="2263320"/>
+          <a:off x="3192120" y="3926160"/>
+          <a:ext cx="6642720" cy="2262960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1150,7 +1147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1161,14 +1158,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
@@ -1403,50 +1400,50 @@
       </c>
     </row>
     <row r="6" s="28" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="29" t="s">
-        <v>43</v>
+      <c r="B6" s="29" t="n">
+        <v>25</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="H6" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="I6" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="J6" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="K6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="L6" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="37" t="s">
+      <c r="M6" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="N6" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="O6" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="P6" s="41" t="s">
         <v>54</v>
-      </c>
-      <c r="P6" s="41" t="s">
-        <v>55</v>
       </c>
       <c r="Q6" s="42"/>
       <c r="R6" s="41"/>
@@ -1728,75 +1725,79 @@
     <mergeCell ref="T4:Y4"/>
     <mergeCell ref="Z4:AB4"/>
   </mergeCells>
-  <dataValidations count="16">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:Y14" type="list">
+  <dataValidations count="17">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:Y14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H14" type="list">
-      <formula1>"Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:S9" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:S9" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AB6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AB6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="decimal">
       <formula1>10</formula1>
       <formula2>400</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q7:Q14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q7:Q14" type="decimal">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6" type="decimal">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G14" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6 S10:S14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6 S10:S14" type="decimal">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B70" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1807,17 +1808,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -1825,10 +1826,10 @@
   <sheetData>
     <row r="1" s="59" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,7 +1845,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1853,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +1861,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,7 +1869,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,13 +1877,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
spreadsheet updates, linkam updates, initial testing with 2021-2 collection
</commit_message>
<xml_diff>
--- a/startup/linkam_template.xlsx
+++ b/startup/linkam_template.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t xml:space="preserve">Linkam</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">Temperature (Celsius)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settling time (seconds)</t>
   </si>
   <si>
     <t xml:space="preserve">Measure this temperature?</t>
@@ -569,7 +572,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,8 +605,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -887,15 +894,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>122760</xdr:colOff>
+      <xdr:colOff>416160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>326160</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:colOff>1139400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -905,7 +912,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3192840" y="3926160"/>
-          <a:ext cx="6643440" cy="2262600"/>
+          <a:ext cx="6643800" cy="1792800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1039,7 +1046,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>5. Specify motor/slit positions in columns Q,R; leave blank for no motion</a:t>
+            <a:t>5. Specify motor/slit positions in columns R,S; leave blank for no motion</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1058,7 +1065,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>6. Specify detector position in column S, blank means to </a:t>
+            <a:t>6. Specify detector position in column T, blank means to </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -1114,26 +1121,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. Do not add columns before column AB</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>l</a:t>
+            <a:t>7. Do not add columns before column AD</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1147,40 +1135,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AMJ14"/>
+  <dimension ref="B1:AC14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="AC7" activeCellId="0" sqref="AC7"/>
+      <selection pane="bottomRight" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="29.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="20" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="26" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1212,8 +1199,9 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1232,92 +1220,94 @@
       <c r="J2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="0"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="U2" s="11"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
-      <c r="Y2" s="10"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
       <c r="T3" s="10"/>
-      <c r="U3" s="0"/>
+      <c r="U3" s="11"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
-      <c r="Y3" s="10"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15" t="s">
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15" t="s">
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15" t="s">
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="16" t="s">
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-    </row>
-    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17" t="s">
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -1326,16 +1316,16 @@
       <c r="D5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="21" t="s">
@@ -1347,75 +1337,78 @@
       <c r="K5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="20" t="s">
         <v>30</v>
       </c>
       <c r="Q5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="R5" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="S5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="T5" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="17" t="s">
+      <c r="U5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="17" t="s">
+      <c r="V5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W5" s="17" t="s">
+      <c r="W5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="X5" s="17" t="s">
+      <c r="X5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="Y5" s="22" t="s">
+      <c r="Y5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="Z5" s="20" t="s">
+      <c r="Z5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AA5" s="27" t="s">
+      <c r="AA5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="AB5" s="27" t="s">
+      <c r="AB5" s="28" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" s="28" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="29" t="n">
+      <c r="AC5" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" s="29" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="30" t="n">
         <v>25</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="30" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="29" t="n">
+      <c r="E6" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="30" t="s">
         <v>45</v>
       </c>
       <c r="H6" s="33" t="s">
@@ -1445,26 +1438,25 @@
       <c r="P6" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="43" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="Q6" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="43"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
       <c r="U6" s="44" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="44" t="n">
+      <c r="V6" s="45" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="44" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="X6" s="44" t="n">
+      <c r="W6" s="45" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="X6" s="45" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1472,242 +1464,253 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="46"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AMJ6" s="0"/>
+      <c r="Z6" s="46" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="47"/>
+      <c r="AB6" s="42"/>
+      <c r="AC6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="47" t="n">
+      <c r="B7" s="48" t="n">
         <v>25</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="51"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="53"/>
-      <c r="S7" s="54"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="54"/>
       <c r="T7" s="55"/>
       <c r="U7" s="56"/>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
-      <c r="X7" s="56"/>
+      <c r="V7" s="57"/>
+      <c r="W7" s="57"/>
+      <c r="X7" s="57"/>
       <c r="Y7" s="57"/>
       <c r="Z7" s="58"/>
+      <c r="AA7" s="59"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="47" t="n">
+      <c r="B8" s="48" t="n">
         <v>100</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="51"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="53"/>
-      <c r="S8" s="54"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="54"/>
       <c r="T8" s="55"/>
       <c r="U8" s="56"/>
-      <c r="V8" s="56"/>
-      <c r="W8" s="56"/>
-      <c r="X8" s="56"/>
+      <c r="V8" s="57"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
       <c r="Y8" s="57"/>
       <c r="Z8" s="58"/>
+      <c r="AA8" s="59"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="47" t="n">
+      <c r="B9" s="48" t="n">
         <v>150</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="48"/>
+      <c r="D9" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="50"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="51"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="53"/>
-      <c r="S9" s="54"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="54"/>
       <c r="T9" s="55"/>
       <c r="U9" s="56"/>
-      <c r="V9" s="56"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="56"/>
+      <c r="V9" s="57"/>
+      <c r="W9" s="57"/>
+      <c r="X9" s="57"/>
       <c r="Y9" s="57"/>
       <c r="Z9" s="58"/>
+      <c r="AA9" s="59"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="47" t="n">
+      <c r="B10" s="48" t="n">
         <v>200</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="50"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="51"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="53"/>
-      <c r="S10" s="54"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="54"/>
       <c r="T10" s="55"/>
       <c r="U10" s="56"/>
-      <c r="V10" s="56"/>
-      <c r="W10" s="56"/>
-      <c r="X10" s="56"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
       <c r="Y10" s="57"/>
       <c r="Z10" s="58"/>
+      <c r="AA10" s="59"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="47" t="n">
+      <c r="B11" s="48" t="n">
         <v>250</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="50"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="51"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="53"/>
-      <c r="S11" s="54"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="54"/>
       <c r="T11" s="55"/>
       <c r="U11" s="56"/>
-      <c r="V11" s="56"/>
-      <c r="W11" s="56"/>
-      <c r="X11" s="56"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
       <c r="Y11" s="57"/>
       <c r="Z11" s="58"/>
+      <c r="AA11" s="59"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="47" t="n">
+      <c r="B12" s="48" t="n">
         <v>300</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="48"/>
+      <c r="D12" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="50"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="51"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="53"/>
-      <c r="S12" s="54"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="54"/>
       <c r="T12" s="55"/>
       <c r="U12" s="56"/>
-      <c r="V12" s="56"/>
-      <c r="W12" s="56"/>
-      <c r="X12" s="56"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
       <c r="Y12" s="57"/>
       <c r="Z12" s="58"/>
+      <c r="AA12" s="59"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="47" t="n">
+      <c r="B13" s="48" t="n">
         <v>350</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="48"/>
+      <c r="D13" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="50"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="51"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="53"/>
-      <c r="S13" s="54"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="54"/>
       <c r="T13" s="55"/>
       <c r="U13" s="56"/>
-      <c r="V13" s="56"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="56"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
       <c r="Y13" s="57"/>
       <c r="Z13" s="58"/>
+      <c r="AA13" s="59"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="47" t="n">
+      <c r="B14" s="48" t="n">
         <v>400</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="50"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="51"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="53"/>
-      <c r="S14" s="54"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="54"/>
       <c r="T14" s="55"/>
       <c r="U14" s="56"/>
-      <c r="V14" s="56"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="56"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
       <c r="Y14" s="57"/>
       <c r="Z14" s="58"/>
+      <c r="AA14" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1716,82 +1719,82 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="T4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="U4:Z4"/>
+    <mergeCell ref="AA4:AC4"/>
   </mergeCells>
   <dataValidations count="17">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:Y14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:Z14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 D6:D14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:S9" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7:T9" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AB6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AA6:AC6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S14" type="decimal">
       <formula1>10</formula1>
       <formula2>400</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q7:Q14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:R14" type="decimal">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="decimal">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6 S10:S14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 T10:T14" type="decimal">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B70" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
-      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+Element at beginning,Temperature+Element at end,Temperature+Element+edge at beginning,Temperature+Element+edge at "</formula1>
+      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1808,7 +1811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1818,18 +1821,18 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
   </cols>
   <sheetData>
-    <row r="1" s="59" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="59" t="s">
+    <row r="1" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="28" t="s">
         <v>56</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,7 +1840,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1864,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,7 +1872,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,7 +1880,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>